<commit_message>
move normalizer options to pattern extraction
</commit_message>
<xml_diff>
--- a/data/normalization.xlsx
+++ b/data/normalization.xlsx
@@ -60172,7 +60172,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -60184,12 +60184,18 @@
       <c r="B1" t="str">
         <v>correct</v>
       </c>
+      <c r="C1" t="str">
+        <v>bel</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>ible\b</v>
       </c>
       <c r="B2" t="str">
+        <v>ible</v>
+      </c>
+      <c r="C2" t="str">
         <v>íbel</v>
       </c>
     </row>
@@ -60198,6 +60204,9 @@
         <v>able\b</v>
       </c>
       <c r="B3" t="str">
+        <v>able</v>
+      </c>
+      <c r="C3" t="str">
         <v>ábel</v>
       </c>
     </row>
@@ -60206,6 +60215,9 @@
         <v>ibles\b</v>
       </c>
       <c r="B4" t="str">
+        <v>ibles</v>
+      </c>
+      <c r="C4" t="str">
         <v>íbeis</v>
       </c>
     </row>
@@ -60214,6 +60226,9 @@
         <v>ables\b</v>
       </c>
       <c r="B5" t="str">
+        <v>ables</v>
+      </c>
+      <c r="C5" t="str">
         <v>ábeis</v>
       </c>
     </row>
@@ -60224,6 +60239,9 @@
       <c r="B6" t="str">
         <v>ece</v>
       </c>
+      <c r="C6" t="str">
+        <v>ece</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -60232,10 +60250,13 @@
       <c r="B7" t="str">
         <v>azo</v>
       </c>
+      <c r="C7" t="str">
+        <v>azo</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>